<commit_message>
data for csc computations
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3657C92D-EFCF-4AC4-97FA-CAC977DD3732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C34A76B-60AC-467B-9678-7C1A6C823BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="1395" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\qgis_derivated_data\mesh\mesh_0.05.msh2</t>
+  </si>
+  <si>
+    <t>graph</t>
+  </si>
+  <si>
+    <t>data/canal_network_matrix_50meters.p</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +515,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
changed read excel to engine='openpyxl'. This was needed for csc to work.
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123C3F66-B439-49CC-9635-BB7D9A15D9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BAA010-2A6E-4380-97CE-C9DBDD6F8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15180" yWindow="4065" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,43 +48,43 @@
     <t>depth</t>
   </si>
   <si>
-    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\qgis_derivated_data\depth_extended.tif</t>
-  </si>
-  <si>
     <t>canal_block_vector</t>
   </si>
   <si>
-    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\0. Raw Data\01. Dam Locations and Data \199_canalblocks_20191008b.shp</t>
-  </si>
-  <si>
-    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\qgis_derivated_data\dtm_depth_padded.tif</t>
-  </si>
-  <si>
     <t>weather_station_coords</t>
   </si>
   <si>
-    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\qgis_derivated_data\weather_station_coordinates.xlsx</t>
-  </si>
-  <si>
     <t>mesh</t>
   </si>
   <si>
     <t>graph</t>
   </si>
   <si>
-    <t>data/canal_network_matrix_50meters.p</t>
-  </si>
-  <si>
     <t>bigger_dem_raster</t>
   </si>
   <si>
-    <t>data\dtm_big_area_depth_padded.tif</t>
-  </si>
-  <si>
     <t>Necessary when the mesh is larger than the DEM and has some cell centers outside of it. If not provided, such mesh would get NaN values!</t>
   </si>
   <si>
-    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2021 SMPP WTD customer work\qgis_derivated_data\mesh\mesh_0.03.msh</t>
+    <t>data/new_area/canal_network_matrix_50meters.p</t>
+  </si>
+  <si>
+    <t>data/new_area/mesh_0.02.msh</t>
+  </si>
+  <si>
+    <t>data/dtm_depth_padded.tif</t>
+  </si>
+  <si>
+    <t>data/depth_extended.tif</t>
+  </si>
+  <si>
+    <t>data/199_canalblocks_20191008b.shp</t>
+  </si>
+  <si>
+    <t>data/weather_station_coordinates.xlsx</t>
+  </si>
+  <si>
+    <t>data/dtm_big_area_depth_padded.tif</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -487,25 +487,25 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -517,29 +517,29 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working before canal line mesh thing
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BAA010-2A6E-4380-97CE-C9DBDD6F8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7A7AC8-375A-4A3E-AC9A-B8AD983A8281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="4065" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="7335" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>data/new_area/canal_network_matrix_50meters.p</t>
   </si>
   <si>
-    <t>data/new_area/mesh_0.02.msh</t>
-  </si>
-  <si>
     <t>data/dtm_depth_padded.tif</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>data/dtm_big_area_depth_padded.tif</t>
+  </si>
+  <si>
+    <t>data/new_area/mesh_0.05.msh</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -487,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -505,7 +505,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -520,7 +520,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
working version of canal lines
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BAA010-2A6E-4380-97CE-C9DBDD6F8B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196B9671-403F-465B-B2E5-266537DE390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="4065" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>data/dtm_big_area_depth_padded.tif</t>
+  </si>
+  <si>
+    <t>channel_network_lines</t>
+  </si>
+  <si>
+    <t>data/new_area/water_bodies_singleparts.gpkg</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,6 +548,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
copied successfully from blopti_dev
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EABC7D1-825C-4A6B-8859-C5C70852AF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3DF797-6E3B-4A2D-A028-B6C7335A2EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>data/new_area/mesh_0.05.msh</t>
+  </si>
+  <si>
+    <t>channel_network_lines</t>
+  </si>
+  <si>
+    <t>data/new_area/water_bodies_singleparts.gpkg</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +549,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
changed files to agree with the version in which canal mesh cells are computed in Qgis
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,19 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3DF797-6E3B-4A2D-A028-B6C7335A2EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6C3F1D-67F4-4E52-AA0C-0F95E4BAE63C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5235" yWindow="4440" windowWidth="9225" windowHeight="10215" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -57,9 +52,6 @@
     <t>mesh</t>
   </si>
   <si>
-    <t>graph</t>
-  </si>
-  <si>
     <t>bigger_dem_raster</t>
   </si>
   <si>
@@ -84,26 +76,36 @@
     <t>data/dtm_big_area_depth_padded.tif</t>
   </si>
   <si>
-    <t>data/new_area/mesh_0.05.msh</t>
-  </si>
-  <si>
-    <t>channel_network_lines</t>
-  </si>
-  <si>
-    <t>data/new_area/water_bodies_singleparts.gpkg</t>
+    <t>channel_network_graph_pickle</t>
+  </si>
+  <si>
+    <t>canal_mask_mesh_centroids</t>
+  </si>
+  <si>
+    <t>data/new_area/mesh_0.035.msh</t>
+  </si>
+  <si>
+    <t>data/new_area/mesh_0.035/canal_mesh_cells.gpkg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -129,15 +131,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{315D8E6C-173D-4E09-8592-58FA30E1B7CF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,7 +458,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -493,7 +499,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -501,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -511,7 +517,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -526,31 +532,31 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="A9" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
+      <c r="A11" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
improved canala ponding: distributed water throughout cell
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC9ECDD-0FB4-4162-B541-4F128EDE20F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB6C3E6-789F-46CE-A733-8DB104CE5C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="5610" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>data/new_area/mesh_0.035/canal_mesh_cells.gpkg</t>
+  </si>
+  <si>
+    <t>initial_zeta_pickle</t>
+  </si>
+  <si>
+    <t>template_output_raster</t>
+  </si>
+  <si>
+    <t>data/new_area/best_initial_zeta.p</t>
   </si>
 </sst>
 </file>
@@ -446,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -542,6 +551,22 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
read Sultan Thaha airport data
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\paper2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB6C3E6-789F-46CE-A733-8DB104CE5C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDC122-5AFA-4215-8D3D-E13BE02049D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5145" yWindow="5610" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12810" yWindow="4395" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>data/new_area/best_initial_zeta.p</t>
+  </si>
+  <si>
+    <t>data/new_area/new_area_dtm.tif</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulation of params 3
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">DEM</t>
   </si>
   <si>
-    <t xml:space="preserve">data/dtm_depth_padded.tif</t>
+    <t xml:space="preserve">data/dtm_depth_padded_filled.tif</t>
   </si>
   <si>
     <t xml:space="preserve">input</t>
@@ -202,10 +202,10 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.28"/>

</xml_diff>